<commit_message>
PDMatlab, um pouco de erro de ss, PMat errado
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leonardo\Desktop\4 ano\Orientada a obeto\ProjetoSemestral\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A776744F-BCD0-4F7E-A2E6-410D92928D6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCA20BAA-E93B-4969-B635-0EF2EEC112AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{C03263EB-8750-4946-8F22-03F56D2BE8A1}"/>
   </bookViews>
@@ -15897,304 +15897,304 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20</c:v>
+                  <c:v>0.02</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>50</c:v>
+                  <c:v>0.05</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>60</c:v>
+                  <c:v>0.06</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>70</c:v>
+                  <c:v>7.0000000000000007E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>80</c:v>
+                  <c:v>0.08</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>90</c:v>
+                  <c:v>0.09</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>100</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>110</c:v>
+                  <c:v>0.11</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>120</c:v>
+                  <c:v>0.12</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>130</c:v>
+                  <c:v>0.13</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>140</c:v>
+                  <c:v>0.14000000000000001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>150</c:v>
+                  <c:v>0.15</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>160</c:v>
+                  <c:v>0.16</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>170</c:v>
+                  <c:v>0.17</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>180</c:v>
+                  <c:v>0.18</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>190</c:v>
+                  <c:v>0.19</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>200</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>210</c:v>
+                  <c:v>0.21</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>220</c:v>
+                  <c:v>0.22</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>230</c:v>
+                  <c:v>0.23</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>240</c:v>
+                  <c:v>0.24</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>250</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>260</c:v>
+                  <c:v>0.26</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>270</c:v>
+                  <c:v>0.27</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>280</c:v>
+                  <c:v>0.28000000000000003</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>290</c:v>
+                  <c:v>0.28999999999999998</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>300</c:v>
+                  <c:v>0.3</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>310</c:v>
+                  <c:v>0.31</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>320</c:v>
+                  <c:v>0.32</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>330</c:v>
+                  <c:v>0.33</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>340</c:v>
+                  <c:v>0.34</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>350</c:v>
+                  <c:v>0.35</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>360</c:v>
+                  <c:v>0.36</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>370</c:v>
+                  <c:v>0.37</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>380</c:v>
+                  <c:v>0.38</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>390</c:v>
+                  <c:v>0.39</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>400</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>410</c:v>
+                  <c:v>0.41</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>420</c:v>
+                  <c:v>0.42</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>430</c:v>
+                  <c:v>0.43</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>440</c:v>
+                  <c:v>0.44</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>450</c:v>
+                  <c:v>0.45</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>460</c:v>
+                  <c:v>0.46</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>470</c:v>
+                  <c:v>0.47</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>480</c:v>
+                  <c:v>0.48</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>490</c:v>
+                  <c:v>0.49</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>500</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>510</c:v>
+                  <c:v>0.51</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>520</c:v>
+                  <c:v>0.52</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>530</c:v>
+                  <c:v>0.53</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>540</c:v>
+                  <c:v>0.54</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>550</c:v>
+                  <c:v>0.55000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>560</c:v>
+                  <c:v>0.56000000000000005</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>570</c:v>
+                  <c:v>0.56999999999999995</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>580</c:v>
+                  <c:v>0.57999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>590</c:v>
+                  <c:v>0.59</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>600</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>610</c:v>
+                  <c:v>0.61</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>620</c:v>
+                  <c:v>0.62</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>630</c:v>
+                  <c:v>0.63</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>640</c:v>
+                  <c:v>0.64</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>650</c:v>
+                  <c:v>0.65</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>660</c:v>
+                  <c:v>0.66</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>670</c:v>
+                  <c:v>0.67</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>680</c:v>
+                  <c:v>0.68</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>690</c:v>
+                  <c:v>0.69</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>700</c:v>
+                  <c:v>0.7</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>710</c:v>
+                  <c:v>0.71</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>720</c:v>
+                  <c:v>0.72</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>730</c:v>
+                  <c:v>0.73</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>740</c:v>
+                  <c:v>0.74</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>750</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>760</c:v>
+                  <c:v>0.76</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>770</c:v>
+                  <c:v>0.77</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>780</c:v>
+                  <c:v>0.78</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>790</c:v>
+                  <c:v>0.79</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>800</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>810</c:v>
+                  <c:v>0.81</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>820</c:v>
+                  <c:v>0.82</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>830</c:v>
+                  <c:v>0.83</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>840</c:v>
+                  <c:v>0.84</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>850</c:v>
+                  <c:v>0.85</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>860</c:v>
+                  <c:v>0.86</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>870</c:v>
+                  <c:v>0.87</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>880</c:v>
+                  <c:v>0.88</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>890</c:v>
+                  <c:v>0.89</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>900</c:v>
+                  <c:v>0.9</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>910</c:v>
+                  <c:v>0.91</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>920</c:v>
+                  <c:v>0.92</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>930</c:v>
+                  <c:v>0.93</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>940</c:v>
+                  <c:v>0.94</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>950</c:v>
+                  <c:v>0.95</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>960</c:v>
+                  <c:v>0.96</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>970</c:v>
+                  <c:v>0.97</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>980</c:v>
+                  <c:v>0.98</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>990</c:v>
+                  <c:v>0.99</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>1000</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -16553,304 +16553,304 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20</c:v>
+                  <c:v>0.02</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30</c:v>
+                  <c:v>0.03</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>50</c:v>
+                  <c:v>0.05</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>60</c:v>
+                  <c:v>0.06</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>70</c:v>
+                  <c:v>7.0000000000000007E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>80</c:v>
+                  <c:v>0.08</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>90</c:v>
+                  <c:v>0.09</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>100</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>110</c:v>
+                  <c:v>0.11</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>120</c:v>
+                  <c:v>0.12</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>130</c:v>
+                  <c:v>0.13</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>140</c:v>
+                  <c:v>0.14000000000000001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>150</c:v>
+                  <c:v>0.15</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>160</c:v>
+                  <c:v>0.16</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>170</c:v>
+                  <c:v>0.17</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>180</c:v>
+                  <c:v>0.18</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>190</c:v>
+                  <c:v>0.19</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>200</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>210</c:v>
+                  <c:v>0.21</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>220</c:v>
+                  <c:v>0.22</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>230</c:v>
+                  <c:v>0.23</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>240</c:v>
+                  <c:v>0.24</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>250</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>260</c:v>
+                  <c:v>0.26</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>270</c:v>
+                  <c:v>0.27</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>280</c:v>
+                  <c:v>0.28000000000000003</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>290</c:v>
+                  <c:v>0.28999999999999998</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>300</c:v>
+                  <c:v>0.3</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>310</c:v>
+                  <c:v>0.31</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>320</c:v>
+                  <c:v>0.32</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>330</c:v>
+                  <c:v>0.33</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>340</c:v>
+                  <c:v>0.34</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>350</c:v>
+                  <c:v>0.35</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>360</c:v>
+                  <c:v>0.36</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>370</c:v>
+                  <c:v>0.37</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>380</c:v>
+                  <c:v>0.38</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>390</c:v>
+                  <c:v>0.39</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>400</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>410</c:v>
+                  <c:v>0.41</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>420</c:v>
+                  <c:v>0.42</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>430</c:v>
+                  <c:v>0.43</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>440</c:v>
+                  <c:v>0.44</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>450</c:v>
+                  <c:v>0.45</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>460</c:v>
+                  <c:v>0.46</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>470</c:v>
+                  <c:v>0.47</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>480</c:v>
+                  <c:v>0.48</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>490</c:v>
+                  <c:v>0.49</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>500</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>510</c:v>
+                  <c:v>0.51</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>520</c:v>
+                  <c:v>0.52</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>530</c:v>
+                  <c:v>0.53</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>540</c:v>
+                  <c:v>0.54</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>550</c:v>
+                  <c:v>0.55000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>560</c:v>
+                  <c:v>0.56000000000000005</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>570</c:v>
+                  <c:v>0.56999999999999995</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>580</c:v>
+                  <c:v>0.57999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>590</c:v>
+                  <c:v>0.59</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>600</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>610</c:v>
+                  <c:v>0.61</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>620</c:v>
+                  <c:v>0.62</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>630</c:v>
+                  <c:v>0.63</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>640</c:v>
+                  <c:v>0.64</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>650</c:v>
+                  <c:v>0.65</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>660</c:v>
+                  <c:v>0.66</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>670</c:v>
+                  <c:v>0.67</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>680</c:v>
+                  <c:v>0.68</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>690</c:v>
+                  <c:v>0.69</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>700</c:v>
+                  <c:v>0.7</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>710</c:v>
+                  <c:v>0.71</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>720</c:v>
+                  <c:v>0.72</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>730</c:v>
+                  <c:v>0.73</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>740</c:v>
+                  <c:v>0.74</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>750</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>760</c:v>
+                  <c:v>0.76</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>770</c:v>
+                  <c:v>0.77</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>780</c:v>
+                  <c:v>0.78</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>790</c:v>
+                  <c:v>0.79</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>800</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>810</c:v>
+                  <c:v>0.81</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>820</c:v>
+                  <c:v>0.82</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>830</c:v>
+                  <c:v>0.83</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>840</c:v>
+                  <c:v>0.84</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>850</c:v>
+                  <c:v>0.85</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>860</c:v>
+                  <c:v>0.86</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>870</c:v>
+                  <c:v>0.87</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>880</c:v>
+                  <c:v>0.88</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>890</c:v>
+                  <c:v>0.89</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>900</c:v>
+                  <c:v>0.9</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>910</c:v>
+                  <c:v>0.91</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>920</c:v>
+                  <c:v>0.92</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>930</c:v>
+                  <c:v>0.93</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>940</c:v>
+                  <c:v>0.94</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>950</c:v>
+                  <c:v>0.95</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>960</c:v>
+                  <c:v>0.96</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>970</c:v>
+                  <c:v>0.97</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>980</c:v>
+                  <c:v>0.98</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>990</c:v>
+                  <c:v>0.99</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>1000</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -16883,7 +16883,7 @@
                   <c:v>728.04</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>849.38</c:v>
+                  <c:v>849.38000000000011</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>970.72</c:v>
@@ -16904,7 +16904,7 @@
                   <c:v>1577.42</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1698.76</c:v>
+                  <c:v>1698.7600000000002</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>1820.1</c:v>
@@ -16943,13 +16943,13 @@
                   <c:v>3154.84</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>3276.18</c:v>
+                  <c:v>3276.1800000000003</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>3397.52</c:v>
+                  <c:v>3397.5200000000004</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>3518.86</c:v>
+                  <c:v>3518.8599999999997</c:v>
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>3640.2</c:v>
@@ -16961,7 +16961,7 @@
                   <c:v>3882.88</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>4004.22</c:v>
+                  <c:v>4004.2200000000003</c:v>
                 </c:pt>
                 <c:pt idx="34">
                   <c:v>4125.5600000000004</c:v>
@@ -17024,22 +17024,22 @@
                   <c:v>6431.02</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>6552.36</c:v>
+                  <c:v>6552.3600000000006</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>6673.7</c:v>
+                  <c:v>6673.7000000000007</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>6795.04</c:v>
+                  <c:v>6795.0400000000009</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>6916.38</c:v>
+                  <c:v>6916.3799999999992</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>7037.72</c:v>
+                  <c:v>7037.7199999999993</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>7159.06</c:v>
+                  <c:v>7159.0599999999995</c:v>
                 </c:pt>
                 <c:pt idx="60">
                   <c:v>7280.4</c:v>
@@ -17060,10 +17060,10 @@
                   <c:v>7887.1</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>8008.44</c:v>
+                  <c:v>8008.4400000000005</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>8129.78</c:v>
+                  <c:v>8129.7800000000007</c:v>
                 </c:pt>
                 <c:pt idx="68">
                   <c:v>8251.1200000000008</c:v>
@@ -19115,16 +19115,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>247649</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>57149</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>42862</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>561974</xdr:colOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>371473</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>33338</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -33627,8 +33627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCFCFF2E-3E9E-4523-9568-A75F41B9794E}">
   <dimension ref="A1:H201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I5" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33692,7 +33692,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>10</v>
+        <v>0.01</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -33719,7 +33719,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>20</v>
+        <v>0.02</v>
       </c>
       <c r="B4">
         <v>4</v>
@@ -33746,7 +33746,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>30</v>
+        <v>0.03</v>
       </c>
       <c r="B5">
         <v>7</v>
@@ -33773,7 +33773,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>40</v>
+        <v>0.04</v>
       </c>
       <c r="B6">
         <v>11</v>
@@ -33800,7 +33800,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>50</v>
+        <v>0.05</v>
       </c>
       <c r="B7">
         <v>16</v>
@@ -33827,7 +33827,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>60</v>
+        <v>0.06</v>
       </c>
       <c r="B8">
         <v>23</v>
@@ -33854,7 +33854,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>70</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="B9">
         <v>29</v>
@@ -33876,12 +33876,12 @@
       </c>
       <c r="H9">
         <f>Tabela3[[#This Row],[Time]]*($G$52-$G$152)/($A$52-$A$152)</f>
-        <v>849.38</v>
+        <v>849.38000000000011</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>80</v>
+        <v>0.08</v>
       </c>
       <c r="B10">
         <v>36</v>
@@ -33908,7 +33908,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>90</v>
+        <v>0.09</v>
       </c>
       <c r="B11">
         <v>44</v>
@@ -33935,7 +33935,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>100</v>
+        <v>0.1</v>
       </c>
       <c r="B12">
         <v>53</v>
@@ -33962,7 +33962,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>110</v>
+        <v>0.11</v>
       </c>
       <c r="B13">
         <v>62</v>
@@ -33989,7 +33989,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>120</v>
+        <v>0.12</v>
       </c>
       <c r="B14">
         <v>72</v>
@@ -34016,7 +34016,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>130</v>
+        <v>0.13</v>
       </c>
       <c r="B15">
         <v>82</v>
@@ -34043,7 +34043,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>140</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="B16">
         <v>93</v>
@@ -34065,12 +34065,12 @@
       </c>
       <c r="H16">
         <f>Tabela3[[#This Row],[Time]]*($G$52-$G$152)/($A$52-$A$152)</f>
-        <v>1698.76</v>
+        <v>1698.7600000000002</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>150</v>
+        <v>0.15</v>
       </c>
       <c r="B17">
         <v>104</v>
@@ -34097,7 +34097,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>160</v>
+        <v>0.16</v>
       </c>
       <c r="B18">
         <v>116</v>
@@ -34124,7 +34124,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>170</v>
+        <v>0.17</v>
       </c>
       <c r="B19">
         <v>129</v>
@@ -34151,7 +34151,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>180</v>
+        <v>0.18</v>
       </c>
       <c r="B20">
         <v>140</v>
@@ -34178,7 +34178,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>190</v>
+        <v>0.19</v>
       </c>
       <c r="B21">
         <v>153</v>
@@ -34205,7 +34205,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>200</v>
+        <v>0.2</v>
       </c>
       <c r="B22">
         <v>166</v>
@@ -34232,7 +34232,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>210</v>
+        <v>0.21</v>
       </c>
       <c r="B23">
         <v>179</v>
@@ -34259,7 +34259,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>220</v>
+        <v>0.22</v>
       </c>
       <c r="B24">
         <v>192</v>
@@ -34286,7 +34286,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>230</v>
+        <v>0.23</v>
       </c>
       <c r="B25">
         <v>206</v>
@@ -34313,7 +34313,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>240</v>
+        <v>0.24</v>
       </c>
       <c r="B26">
         <v>220</v>
@@ -34340,7 +34340,7 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>250</v>
+        <v>0.25</v>
       </c>
       <c r="B27">
         <v>235</v>
@@ -34367,7 +34367,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>260</v>
+        <v>0.26</v>
       </c>
       <c r="B28">
         <v>249</v>
@@ -34394,7 +34394,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>270</v>
+        <v>0.27</v>
       </c>
       <c r="B29">
         <v>264</v>
@@ -34416,12 +34416,12 @@
       </c>
       <c r="H29">
         <f>Tabela3[[#This Row],[Time]]*($G$52-$G$152)/($A$52-$A$152)</f>
-        <v>3276.18</v>
+        <v>3276.1800000000003</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>280</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="B30">
         <v>279</v>
@@ -34443,12 +34443,12 @@
       </c>
       <c r="H30">
         <f>Tabela3[[#This Row],[Time]]*($G$52-$G$152)/($A$52-$A$152)</f>
-        <v>3397.52</v>
+        <v>3397.5200000000004</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>290</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="B31">
         <v>294</v>
@@ -34470,12 +34470,12 @@
       </c>
       <c r="H31">
         <f>Tabela3[[#This Row],[Time]]*($G$52-$G$152)/($A$52-$A$152)</f>
-        <v>3518.86</v>
+        <v>3518.8599999999997</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>300</v>
+        <v>0.3</v>
       </c>
       <c r="B32">
         <v>308</v>
@@ -34502,7 +34502,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>310</v>
+        <v>0.31</v>
       </c>
       <c r="B33">
         <v>325</v>
@@ -34529,7 +34529,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>320</v>
+        <v>0.32</v>
       </c>
       <c r="B34">
         <v>341</v>
@@ -34556,7 +34556,7 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>330</v>
+        <v>0.33</v>
       </c>
       <c r="B35">
         <v>357</v>
@@ -34578,12 +34578,12 @@
       </c>
       <c r="H35">
         <f>Tabela3[[#This Row],[Time]]*($G$52-$G$152)/($A$52-$A$152)</f>
-        <v>4004.22</v>
+        <v>4004.2200000000003</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>340</v>
+        <v>0.34</v>
       </c>
       <c r="B36">
         <v>372</v>
@@ -34610,7 +34610,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>350</v>
+        <v>0.35</v>
       </c>
       <c r="B37">
         <v>388</v>
@@ -34637,7 +34637,7 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>360</v>
+        <v>0.36</v>
       </c>
       <c r="B38">
         <v>405</v>
@@ -34664,7 +34664,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>370</v>
+        <v>0.37</v>
       </c>
       <c r="B39">
         <v>422</v>
@@ -34691,7 +34691,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>380</v>
+        <v>0.38</v>
       </c>
       <c r="B40">
         <v>437</v>
@@ -34718,7 +34718,7 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>390</v>
+        <v>0.39</v>
       </c>
       <c r="B41">
         <v>454</v>
@@ -34745,7 +34745,7 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>400</v>
+        <v>0.4</v>
       </c>
       <c r="B42">
         <v>471</v>
@@ -34772,7 +34772,7 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>410</v>
+        <v>0.41</v>
       </c>
       <c r="B43">
         <v>489</v>
@@ -34799,7 +34799,7 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>420</v>
+        <v>0.42</v>
       </c>
       <c r="B44">
         <v>505</v>
@@ -34826,7 +34826,7 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>430</v>
+        <v>0.43</v>
       </c>
       <c r="B45">
         <v>523</v>
@@ -34853,7 +34853,7 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>440</v>
+        <v>0.44</v>
       </c>
       <c r="B46">
         <v>540</v>
@@ -34880,7 +34880,7 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>450</v>
+        <v>0.45</v>
       </c>
       <c r="B47">
         <v>558</v>
@@ -34907,7 +34907,7 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>460</v>
+        <v>0.46</v>
       </c>
       <c r="B48">
         <v>576</v>
@@ -34934,7 +34934,7 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>470</v>
+        <v>0.47</v>
       </c>
       <c r="B49">
         <v>594</v>
@@ -34961,7 +34961,7 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>480</v>
+        <v>0.48</v>
       </c>
       <c r="B50">
         <v>612</v>
@@ -34988,7 +34988,7 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>490</v>
+        <v>0.49</v>
       </c>
       <c r="B51">
         <v>629</v>
@@ -35015,7 +35015,7 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>500</v>
+        <v>0.5</v>
       </c>
       <c r="B52">
         <v>647</v>
@@ -35042,7 +35042,7 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>510</v>
+        <v>0.51</v>
       </c>
       <c r="B53">
         <v>665</v>
@@ -35069,7 +35069,7 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>520</v>
+        <v>0.52</v>
       </c>
       <c r="B54">
         <v>684</v>
@@ -35096,7 +35096,7 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>530</v>
+        <v>0.53</v>
       </c>
       <c r="B55">
         <v>700</v>
@@ -35123,7 +35123,7 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>540</v>
+        <v>0.54</v>
       </c>
       <c r="B56">
         <v>719</v>
@@ -35145,12 +35145,12 @@
       </c>
       <c r="H56">
         <f>Tabela3[[#This Row],[Time]]*($G$52-$G$152)/($A$52-$A$152)</f>
-        <v>6552.36</v>
+        <v>6552.3600000000006</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>550</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="B57">
         <v>738</v>
@@ -35172,12 +35172,12 @@
       </c>
       <c r="H57">
         <f>Tabela3[[#This Row],[Time]]*($G$52-$G$152)/($A$52-$A$152)</f>
-        <v>6673.7</v>
+        <v>6673.7000000000007</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>560</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="B58">
         <v>756</v>
@@ -35199,12 +35199,12 @@
       </c>
       <c r="H58">
         <f>Tabela3[[#This Row],[Time]]*($G$52-$G$152)/($A$52-$A$152)</f>
-        <v>6795.04</v>
+        <v>6795.0400000000009</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>570</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="B59">
         <v>773</v>
@@ -35226,12 +35226,12 @@
       </c>
       <c r="H59">
         <f>Tabela3[[#This Row],[Time]]*($G$52-$G$152)/($A$52-$A$152)</f>
-        <v>6916.38</v>
+        <v>6916.3799999999992</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>580</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="B60">
         <v>792</v>
@@ -35253,12 +35253,12 @@
       </c>
       <c r="H60">
         <f>Tabela3[[#This Row],[Time]]*($G$52-$G$152)/($A$52-$A$152)</f>
-        <v>7037.72</v>
+        <v>7037.7199999999993</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>590</v>
+        <v>0.59</v>
       </c>
       <c r="B61">
         <v>811</v>
@@ -35280,12 +35280,12 @@
       </c>
       <c r="H61">
         <f>Tabela3[[#This Row],[Time]]*($G$52-$G$152)/($A$52-$A$152)</f>
-        <v>7159.06</v>
+        <v>7159.0599999999995</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>600</v>
+        <v>0.6</v>
       </c>
       <c r="B62">
         <v>829</v>
@@ -35312,7 +35312,7 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>610</v>
+        <v>0.61</v>
       </c>
       <c r="B63">
         <v>847</v>
@@ -35339,7 +35339,7 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>620</v>
+        <v>0.62</v>
       </c>
       <c r="B64">
         <v>866</v>
@@ -35366,7 +35366,7 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>630</v>
+        <v>0.63</v>
       </c>
       <c r="B65">
         <v>885</v>
@@ -35393,7 +35393,7 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>640</v>
+        <v>0.64</v>
       </c>
       <c r="B66">
         <v>904</v>
@@ -35420,7 +35420,7 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>650</v>
+        <v>0.65</v>
       </c>
       <c r="B67">
         <v>921</v>
@@ -35447,7 +35447,7 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>660</v>
+        <v>0.66</v>
       </c>
       <c r="B68">
         <v>940</v>
@@ -35469,12 +35469,12 @@
       </c>
       <c r="H68">
         <f>Tabela3[[#This Row],[Time]]*($G$52-$G$152)/($A$52-$A$152)</f>
-        <v>8008.44</v>
+        <v>8008.4400000000005</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>670</v>
+        <v>0.67</v>
       </c>
       <c r="B69">
         <v>960</v>
@@ -35496,12 +35496,12 @@
       </c>
       <c r="H69">
         <f>Tabela3[[#This Row],[Time]]*($G$52-$G$152)/($A$52-$A$152)</f>
-        <v>8129.78</v>
+        <v>8129.7800000000007</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>680</v>
+        <v>0.68</v>
       </c>
       <c r="B70">
         <v>979</v>
@@ -35528,7 +35528,7 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>690</v>
+        <v>0.69</v>
       </c>
       <c r="B71">
         <v>996</v>
@@ -35555,7 +35555,7 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>700</v>
+        <v>0.7</v>
       </c>
       <c r="B72">
         <v>1016</v>
@@ -35582,7 +35582,7 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>710</v>
+        <v>0.71</v>
       </c>
       <c r="B73">
         <v>1035</v>
@@ -35609,7 +35609,7 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>720</v>
+        <v>0.72</v>
       </c>
       <c r="B74">
         <v>1055</v>
@@ -35636,7 +35636,7 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>730</v>
+        <v>0.73</v>
       </c>
       <c r="B75">
         <v>1075</v>
@@ -35663,7 +35663,7 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>740</v>
+        <v>0.74</v>
       </c>
       <c r="B76">
         <v>1094</v>
@@ -35690,7 +35690,7 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>750</v>
+        <v>0.75</v>
       </c>
       <c r="B77">
         <v>1114</v>
@@ -35717,7 +35717,7 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>760</v>
+        <v>0.76</v>
       </c>
       <c r="B78">
         <v>1132</v>
@@ -35744,7 +35744,7 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>770</v>
+        <v>0.77</v>
       </c>
       <c r="B79">
         <v>1151</v>
@@ -35771,7 +35771,7 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>780</v>
+        <v>0.78</v>
       </c>
       <c r="B80">
         <v>1171</v>
@@ -35798,7 +35798,7 @@
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>790</v>
+        <v>0.79</v>
       </c>
       <c r="B81">
         <v>1191</v>
@@ -35825,7 +35825,7 @@
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>800</v>
+        <v>0.8</v>
       </c>
       <c r="B82">
         <v>1209</v>
@@ -35852,7 +35852,7 @@
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>810</v>
+        <v>0.81</v>
       </c>
       <c r="B83">
         <v>1229</v>
@@ -35879,7 +35879,7 @@
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>820</v>
+        <v>0.82</v>
       </c>
       <c r="B84">
         <v>1249</v>
@@ -35906,7 +35906,7 @@
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>830</v>
+        <v>0.83</v>
       </c>
       <c r="B85">
         <v>1269</v>
@@ -35933,7 +35933,7 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>840</v>
+        <v>0.84</v>
       </c>
       <c r="B86">
         <v>1287</v>
@@ -35960,7 +35960,7 @@
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>850</v>
+        <v>0.85</v>
       </c>
       <c r="B87">
         <v>1307</v>
@@ -35987,7 +35987,7 @@
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>860</v>
+        <v>0.86</v>
       </c>
       <c r="B88">
         <v>1327</v>
@@ -36014,7 +36014,7 @@
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>870</v>
+        <v>0.87</v>
       </c>
       <c r="B89">
         <v>1347</v>
@@ -36041,7 +36041,7 @@
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>880</v>
+        <v>0.88</v>
       </c>
       <c r="B90">
         <v>1366</v>
@@ -36068,7 +36068,7 @@
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>890</v>
+        <v>0.89</v>
       </c>
       <c r="B91">
         <v>1386</v>
@@ -36095,7 +36095,7 @@
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>900</v>
+        <v>0.9</v>
       </c>
       <c r="B92">
         <v>1406</v>
@@ -36122,7 +36122,7 @@
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>910</v>
+        <v>0.91</v>
       </c>
       <c r="B93">
         <v>1427</v>
@@ -36149,7 +36149,7 @@
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>920</v>
+        <v>0.92</v>
       </c>
       <c r="B94">
         <v>1445</v>
@@ -36176,7 +36176,7 @@
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>930</v>
+        <v>0.93</v>
       </c>
       <c r="B95">
         <v>1465</v>
@@ -36203,7 +36203,7 @@
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>940</v>
+        <v>0.94</v>
       </c>
       <c r="B96">
         <v>1486</v>
@@ -36230,7 +36230,7 @@
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>950</v>
+        <v>0.95</v>
       </c>
       <c r="B97">
         <v>1506</v>
@@ -36257,7 +36257,7 @@
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>960</v>
+        <v>0.96</v>
       </c>
       <c r="B98">
         <v>1525</v>
@@ -36284,7 +36284,7 @@
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>970</v>
+        <v>0.97</v>
       </c>
       <c r="B99">
         <v>1545</v>
@@ -36311,7 +36311,7 @@
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100">
-        <v>980</v>
+        <v>0.98</v>
       </c>
       <c r="B100">
         <v>1566</v>
@@ -36338,7 +36338,7 @@
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101">
-        <v>990</v>
+        <v>0.99</v>
       </c>
       <c r="B101">
         <v>1586</v>
@@ -36365,7 +36365,7 @@
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102">
-        <v>1000</v>
+        <v>1</v>
       </c>
       <c r="B102">
         <v>1605</v>
@@ -36392,7 +36392,7 @@
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103">
-        <v>1010</v>
+        <v>1.01</v>
       </c>
       <c r="B103">
         <v>1625</v>
@@ -36419,7 +36419,7 @@
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104">
-        <v>1020</v>
+        <v>1.02</v>
       </c>
       <c r="B104">
         <v>1646</v>
@@ -36446,7 +36446,7 @@
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105">
-        <v>1030</v>
+        <v>1.03</v>
       </c>
       <c r="B105">
         <v>1666</v>
@@ -36473,7 +36473,7 @@
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106">
-        <v>1040</v>
+        <v>1.04</v>
       </c>
       <c r="B106">
         <v>1687</v>
@@ -36500,7 +36500,7 @@
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107">
-        <v>1050</v>
+        <v>1.05</v>
       </c>
       <c r="B107">
         <v>1708</v>
@@ -36527,7 +36527,7 @@
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108">
-        <v>1060</v>
+        <v>1.06</v>
       </c>
       <c r="B108">
         <v>1728</v>
@@ -36554,7 +36554,7 @@
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109">
-        <v>1070</v>
+        <v>1.07</v>
       </c>
       <c r="B109">
         <v>1747</v>
@@ -36576,12 +36576,12 @@
       </c>
       <c r="H109">
         <f>Tabela3[[#This Row],[Time]]*($G$52-$G$152)/($A$52-$A$152)</f>
-        <v>12983.38</v>
+        <v>12983.380000000001</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110">
-        <v>1080</v>
+        <v>1.08</v>
       </c>
       <c r="B110">
         <v>1767</v>
@@ -36603,12 +36603,12 @@
       </c>
       <c r="H110">
         <f>Tabela3[[#This Row],[Time]]*($G$52-$G$152)/($A$52-$A$152)</f>
-        <v>13104.72</v>
+        <v>13104.720000000001</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111">
-        <v>1090</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="B111">
         <v>1788</v>
@@ -36630,12 +36630,12 @@
       </c>
       <c r="H111">
         <f>Tabela3[[#This Row],[Time]]*($G$52-$G$152)/($A$52-$A$152)</f>
-        <v>13226.06</v>
+        <v>13226.060000000001</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112">
-        <v>1100</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="B112">
         <v>1809</v>
@@ -36657,12 +36657,12 @@
       </c>
       <c r="H112">
         <f>Tabela3[[#This Row],[Time]]*($G$52-$G$152)/($A$52-$A$152)</f>
-        <v>13347.4</v>
+        <v>13347.400000000001</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113">
-        <v>1110</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="B113">
         <v>1829</v>
@@ -36684,12 +36684,12 @@
       </c>
       <c r="H113">
         <f>Tabela3[[#This Row],[Time]]*($G$52-$G$152)/($A$52-$A$152)</f>
-        <v>13468.74</v>
+        <v>13468.740000000002</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114">
-        <v>1120</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="B114">
         <v>1850</v>
@@ -36711,12 +36711,12 @@
       </c>
       <c r="H114">
         <f>Tabela3[[#This Row],[Time]]*($G$52-$G$152)/($A$52-$A$152)</f>
-        <v>13590.08</v>
+        <v>13590.080000000002</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115">
-        <v>1130</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="B115">
         <v>1870</v>
@@ -36738,12 +36738,12 @@
       </c>
       <c r="H115">
         <f>Tabela3[[#This Row],[Time]]*($G$52-$G$152)/($A$52-$A$152)</f>
-        <v>13711.42</v>
+        <v>13711.419999999998</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116">
-        <v>1140</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="B116">
         <v>1891</v>
@@ -36765,12 +36765,12 @@
       </c>
       <c r="H116">
         <f>Tabela3[[#This Row],[Time]]*($G$52-$G$152)/($A$52-$A$152)</f>
-        <v>13832.76</v>
+        <v>13832.759999999998</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117">
-        <v>1150</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="B117">
         <v>1910</v>
@@ -36792,12 +36792,12 @@
       </c>
       <c r="H117">
         <f>Tabela3[[#This Row],[Time]]*($G$52-$G$152)/($A$52-$A$152)</f>
-        <v>13954.1</v>
+        <v>13954.099999999999</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118">
-        <v>1160</v>
+        <v>1.1599999999999999</v>
       </c>
       <c r="B118">
         <v>1931</v>
@@ -36819,12 +36819,12 @@
       </c>
       <c r="H118">
         <f>Tabela3[[#This Row],[Time]]*($G$52-$G$152)/($A$52-$A$152)</f>
-        <v>14075.44</v>
+        <v>14075.439999999999</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119">
-        <v>1170</v>
+        <v>1.17</v>
       </c>
       <c r="B119">
         <v>1952</v>
@@ -36846,12 +36846,12 @@
       </c>
       <c r="H119">
         <f>Tabela3[[#This Row],[Time]]*($G$52-$G$152)/($A$52-$A$152)</f>
-        <v>14196.78</v>
+        <v>14196.779999999999</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120">
-        <v>1180</v>
+        <v>1.18</v>
       </c>
       <c r="B120">
         <v>1973</v>
@@ -36873,12 +36873,12 @@
       </c>
       <c r="H120">
         <f>Tabela3[[#This Row],[Time]]*($G$52-$G$152)/($A$52-$A$152)</f>
-        <v>14318.12</v>
+        <v>14318.119999999999</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121">
-        <v>1190</v>
+        <v>1.19</v>
       </c>
       <c r="B121">
         <v>1992</v>
@@ -36905,7 +36905,7 @@
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122">
-        <v>1200</v>
+        <v>1.2</v>
       </c>
       <c r="B122">
         <v>2012</v>
@@ -36932,7 +36932,7 @@
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123">
-        <v>1210</v>
+        <v>1.21</v>
       </c>
       <c r="B123">
         <v>2033</v>
@@ -36959,7 +36959,7 @@
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124">
-        <v>1220</v>
+        <v>1.22</v>
       </c>
       <c r="B124">
         <v>2055</v>
@@ -36986,7 +36986,7 @@
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125">
-        <v>1230</v>
+        <v>1.23</v>
       </c>
       <c r="B125">
         <v>2074</v>
@@ -37013,7 +37013,7 @@
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126">
-        <v>1240</v>
+        <v>1.24</v>
       </c>
       <c r="B126">
         <v>2095</v>
@@ -37040,7 +37040,7 @@
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127">
-        <v>1250</v>
+        <v>1.25</v>
       </c>
       <c r="B127">
         <v>2116</v>
@@ -37067,7 +37067,7 @@
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128">
-        <v>1260</v>
+        <v>1.26</v>
       </c>
       <c r="B128">
         <v>2138</v>
@@ -37094,7 +37094,7 @@
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129">
-        <v>1270</v>
+        <v>1.27</v>
       </c>
       <c r="B129">
         <v>2157</v>
@@ -37121,7 +37121,7 @@
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130">
-        <v>1280</v>
+        <v>1.28</v>
       </c>
       <c r="B130">
         <v>2178</v>
@@ -37148,7 +37148,7 @@
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131">
-        <v>1290</v>
+        <v>1.29</v>
       </c>
       <c r="B131">
         <v>2200</v>
@@ -37175,7 +37175,7 @@
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132">
-        <v>1300</v>
+        <v>1.3</v>
       </c>
       <c r="B132">
         <v>2221</v>
@@ -37202,7 +37202,7 @@
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133">
-        <v>1310</v>
+        <v>1.31</v>
       </c>
       <c r="B133">
         <v>2242</v>
@@ -37229,7 +37229,7 @@
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134">
-        <v>1320</v>
+        <v>1.32</v>
       </c>
       <c r="B134">
         <v>2264</v>
@@ -37251,12 +37251,12 @@
       </c>
       <c r="H134">
         <f>Tabela3[[#This Row],[Time]]*($G$52-$G$152)/($A$52-$A$152)</f>
-        <v>16016.88</v>
+        <v>16016.880000000001</v>
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135">
-        <v>1330</v>
+        <v>1.33</v>
       </c>
       <c r="B135">
         <v>2285</v>
@@ -37278,12 +37278,12 @@
       </c>
       <c r="H135">
         <f>Tabela3[[#This Row],[Time]]*($G$52-$G$152)/($A$52-$A$152)</f>
-        <v>16138.22</v>
+        <v>16138.220000000001</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136">
-        <v>1340</v>
+        <v>1.34</v>
       </c>
       <c r="B136">
         <v>2305</v>
@@ -37305,12 +37305,12 @@
       </c>
       <c r="H136">
         <f>Tabela3[[#This Row],[Time]]*($G$52-$G$152)/($A$52-$A$152)</f>
-        <v>16259.56</v>
+        <v>16259.560000000001</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137">
-        <v>1350</v>
+        <v>1.35</v>
       </c>
       <c r="B137">
         <v>2327</v>
@@ -37332,12 +37332,12 @@
       </c>
       <c r="H137">
         <f>Tabela3[[#This Row],[Time]]*($G$52-$G$152)/($A$52-$A$152)</f>
-        <v>16380.9</v>
+        <v>16380.900000000001</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138">
-        <v>1360</v>
+        <v>1.36</v>
       </c>
       <c r="B138">
         <v>2348</v>
@@ -37364,7 +37364,7 @@
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139">
-        <v>1370</v>
+        <v>1.37</v>
       </c>
       <c r="B139">
         <v>2370</v>
@@ -37391,7 +37391,7 @@
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140">
-        <v>1380</v>
+        <v>1.38</v>
       </c>
       <c r="B140">
         <v>2389</v>
@@ -37418,7 +37418,7 @@
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141">
-        <v>1390</v>
+        <v>1.39</v>
       </c>
       <c r="B141">
         <v>2411</v>
@@ -37445,7 +37445,7 @@
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142">
-        <v>1400</v>
+        <v>1.4</v>
       </c>
       <c r="B142">
         <v>2432</v>
@@ -37472,7 +37472,7 @@
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143">
-        <v>1410</v>
+        <v>1.41</v>
       </c>
       <c r="B143">
         <v>2454</v>
@@ -37499,7 +37499,7 @@
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144">
-        <v>1420</v>
+        <v>1.42</v>
       </c>
       <c r="B144">
         <v>2474</v>
@@ -37526,7 +37526,7 @@
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145">
-        <v>1430</v>
+        <v>1.43</v>
       </c>
       <c r="B145">
         <v>2496</v>
@@ -37553,7 +37553,7 @@
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146">
-        <v>1440</v>
+        <v>1.44</v>
       </c>
       <c r="B146">
         <v>2518</v>
@@ -37580,7 +37580,7 @@
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147">
-        <v>1450</v>
+        <v>1.45</v>
       </c>
       <c r="B147">
         <v>2539</v>
@@ -37607,7 +37607,7 @@
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148">
-        <v>1460</v>
+        <v>1.46</v>
       </c>
       <c r="B148">
         <v>2559</v>
@@ -37634,7 +37634,7 @@
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149">
-        <v>1470</v>
+        <v>1.47</v>
       </c>
       <c r="B149">
         <v>2581</v>
@@ -37661,7 +37661,7 @@
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150">
-        <v>1480</v>
+        <v>1.48</v>
       </c>
       <c r="B150">
         <v>2603</v>
@@ -37688,7 +37688,7 @@
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151">
-        <v>1490</v>
+        <v>1.49</v>
       </c>
       <c r="B151">
         <v>2625</v>
@@ -37715,7 +37715,7 @@
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152">
-        <v>1500</v>
+        <v>1.5</v>
       </c>
       <c r="B152">
         <v>2645</v>
@@ -37742,7 +37742,7 @@
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153">
-        <v>1510</v>
+        <v>1.51</v>
       </c>
       <c r="B153">
         <v>2667</v>
@@ -37769,7 +37769,7 @@
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154">
-        <v>1520</v>
+        <v>1.52</v>
       </c>
       <c r="B154">
         <v>2689</v>
@@ -37796,7 +37796,7 @@
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155">
-        <v>1530</v>
+        <v>1.53</v>
       </c>
       <c r="B155">
         <v>2711</v>
@@ -37823,7 +37823,7 @@
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156">
-        <v>1540</v>
+        <v>1.54</v>
       </c>
       <c r="B156">
         <v>2730</v>
@@ -37850,7 +37850,7 @@
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157">
-        <v>1550</v>
+        <v>1.55</v>
       </c>
       <c r="B157">
         <v>2753</v>
@@ -37877,7 +37877,7 @@
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158">
-        <v>1560</v>
+        <v>1.56</v>
       </c>
       <c r="B158">
         <v>2775</v>
@@ -37904,7 +37904,7 @@
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159">
-        <v>1570</v>
+        <v>1.57</v>
       </c>
       <c r="B159">
         <v>2797</v>
@@ -37931,7 +37931,7 @@
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160">
-        <v>1580</v>
+        <v>1.58</v>
       </c>
       <c r="B160">
         <v>2818</v>
@@ -37958,7 +37958,7 @@
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161">
-        <v>1590</v>
+        <v>1.59</v>
       </c>
       <c r="B161">
         <v>2840</v>
@@ -37985,7 +37985,7 @@
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A162">
-        <v>1600</v>
+        <v>1.6</v>
       </c>
       <c r="B162">
         <v>2862</v>
@@ -38012,7 +38012,7 @@
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163">
-        <v>1610</v>
+        <v>1.61</v>
       </c>
       <c r="B163">
         <v>2884</v>
@@ -38039,7 +38039,7 @@
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164">
-        <v>1620</v>
+        <v>1.62</v>
       </c>
       <c r="B164">
         <v>2906</v>
@@ -38066,7 +38066,7 @@
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A165">
-        <v>1630</v>
+        <v>1.63</v>
       </c>
       <c r="B165">
         <v>2928</v>
@@ -38093,7 +38093,7 @@
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A166">
-        <v>1640</v>
+        <v>1.64</v>
       </c>
       <c r="B166">
         <v>2951</v>
@@ -38120,7 +38120,7 @@
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167">
-        <v>1650</v>
+        <v>1.65</v>
       </c>
       <c r="B167">
         <v>2971</v>
@@ -38147,7 +38147,7 @@
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A168">
-        <v>1660</v>
+        <v>1.66</v>
       </c>
       <c r="B168">
         <v>2994</v>
@@ -38174,7 +38174,7 @@
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169">
-        <v>1670</v>
+        <v>1.67</v>
       </c>
       <c r="B169">
         <v>3016</v>
@@ -38201,7 +38201,7 @@
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A170">
-        <v>1680</v>
+        <v>1.68</v>
       </c>
       <c r="B170">
         <v>3038</v>
@@ -38228,7 +38228,7 @@
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171">
-        <v>1690</v>
+        <v>1.69</v>
       </c>
       <c r="B171">
         <v>3059</v>
@@ -38255,7 +38255,7 @@
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A172">
-        <v>1700</v>
+        <v>1.7</v>
       </c>
       <c r="B172">
         <v>3081</v>
@@ -38282,7 +38282,7 @@
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A173">
-        <v>1710</v>
+        <v>1.71</v>
       </c>
       <c r="B173">
         <v>3103</v>
@@ -38309,7 +38309,7 @@
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A174">
-        <v>1720</v>
+        <v>1.72</v>
       </c>
       <c r="B174">
         <v>3126</v>
@@ -38336,7 +38336,7 @@
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A175">
-        <v>1730</v>
+        <v>1.73</v>
       </c>
       <c r="B175">
         <v>3147</v>
@@ -38363,7 +38363,7 @@
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A176">
-        <v>1740</v>
+        <v>1.74</v>
       </c>
       <c r="B176">
         <v>3169</v>
@@ -38390,7 +38390,7 @@
     </row>
     <row r="177" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A177">
-        <v>1750</v>
+        <v>1.75</v>
       </c>
       <c r="B177">
         <v>3191</v>
@@ -38417,7 +38417,7 @@
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A178">
-        <v>1760</v>
+        <v>1.76</v>
       </c>
       <c r="B178">
         <v>3214</v>
@@ -38444,7 +38444,7 @@
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A179">
-        <v>1770</v>
+        <v>1.77</v>
       </c>
       <c r="B179">
         <v>3234</v>
@@ -38471,7 +38471,7 @@
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A180">
-        <v>1780</v>
+        <v>1.78</v>
       </c>
       <c r="B180">
         <v>3257</v>
@@ -38498,7 +38498,7 @@
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A181">
-        <v>1790</v>
+        <v>1.79</v>
       </c>
       <c r="B181">
         <v>3280</v>
@@ -38525,7 +38525,7 @@
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A182">
-        <v>1800</v>
+        <v>1.8</v>
       </c>
       <c r="B182">
         <v>3303</v>
@@ -38552,7 +38552,7 @@
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A183">
-        <v>1810</v>
+        <v>1.81</v>
       </c>
       <c r="B183">
         <v>3323</v>
@@ -38579,7 +38579,7 @@
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A184">
-        <v>1820</v>
+        <v>1.82</v>
       </c>
       <c r="B184">
         <v>3346</v>
@@ -38606,7 +38606,7 @@
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A185">
-        <v>1830</v>
+        <v>1.83</v>
       </c>
       <c r="B185">
         <v>3368</v>
@@ -38633,7 +38633,7 @@
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A186">
-        <v>1840</v>
+        <v>1.84</v>
       </c>
       <c r="B186">
         <v>3391</v>
@@ -38660,7 +38660,7 @@
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A187">
-        <v>1850</v>
+        <v>1.85</v>
       </c>
       <c r="B187">
         <v>3412</v>
@@ -38687,7 +38687,7 @@
     </row>
     <row r="188" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A188">
-        <v>1860</v>
+        <v>1.86</v>
       </c>
       <c r="B188">
         <v>3435</v>
@@ -38714,7 +38714,7 @@
     </row>
     <row r="189" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A189">
-        <v>1870</v>
+        <v>1.87</v>
       </c>
       <c r="B189">
         <v>3458</v>
@@ -38741,7 +38741,7 @@
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A190">
-        <v>1880</v>
+        <v>1.88</v>
       </c>
       <c r="B190">
         <v>3481</v>
@@ -38768,7 +38768,7 @@
     </row>
     <row r="191" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A191">
-        <v>1890</v>
+        <v>1.89</v>
       </c>
       <c r="B191">
         <v>3503</v>
@@ -38795,7 +38795,7 @@
     </row>
     <row r="192" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A192">
-        <v>1900</v>
+        <v>1.9</v>
       </c>
       <c r="B192">
         <v>3526</v>
@@ -38822,7 +38822,7 @@
     </row>
     <row r="193" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A193">
-        <v>1910</v>
+        <v>1.91</v>
       </c>
       <c r="B193">
         <v>3549</v>
@@ -38849,7 +38849,7 @@
     </row>
     <row r="194" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A194">
-        <v>1920</v>
+        <v>1.92</v>
       </c>
       <c r="B194">
         <v>3570</v>
@@ -38876,7 +38876,7 @@
     </row>
     <row r="195" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A195">
-        <v>1930</v>
+        <v>1.93</v>
       </c>
       <c r="B195">
         <v>3593</v>
@@ -38903,7 +38903,7 @@
     </row>
     <row r="196" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A196">
-        <v>1940</v>
+        <v>1.94</v>
       </c>
       <c r="B196">
         <v>3616</v>
@@ -38930,7 +38930,7 @@
     </row>
     <row r="197" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A197">
-        <v>1950</v>
+        <v>1.95</v>
       </c>
       <c r="B197">
         <v>3639</v>
@@ -38957,7 +38957,7 @@
     </row>
     <row r="198" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A198">
-        <v>1960</v>
+        <v>1.96</v>
       </c>
       <c r="B198">
         <v>3660</v>
@@ -38984,7 +38984,7 @@
     </row>
     <row r="199" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A199">
-        <v>1970</v>
+        <v>1.97</v>
       </c>
       <c r="B199">
         <v>3683</v>
@@ -39011,7 +39011,7 @@
     </row>
     <row r="200" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A200">
-        <v>1980</v>
+        <v>1.98</v>
       </c>
       <c r="B200">
         <v>3706</v>
@@ -39038,7 +39038,7 @@
     </row>
     <row r="201" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A201">
-        <v>1990</v>
+        <v>1.99</v>
       </c>
       <c r="B201">
         <v>3729</v>

</xml_diff>